<commit_message>
Updated readme and supporting docs
</commit_message>
<xml_diff>
--- a/00_data/2014_wgs_6x7-F1/supporting_documentation/20140102_A_SeqProduction_Cheng.xlsx
+++ b/00_data/2014_wgs_6x7-F1/supporting_documentation/20140102_A_SeqProduction_Cheng.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28360" yWindow="0" windowWidth="17340" windowHeight="12840" tabRatio="500"/>
+    <workbookView xWindow="-19060" yWindow="100" windowWidth="17340" windowHeight="12840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -390,37 +390,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1216,7 +1186,7 @@
         <v>56364624</v>
       </c>
       <c r="E20" s="12">
-        <f t="shared" ref="E20:E23" si="2">D20/D$22</f>
+        <f t="shared" ref="E20:E21" si="2">D20/D$22</f>
         <v>0.45474505038599089</v>
       </c>
       <c r="F20" s="12">
@@ -4628,12 +4598,12 @@
     <sortCondition ref="B21:B30"/>
   </sortState>
   <conditionalFormatting sqref="A9:H11">
-    <cfRule type="expression" dxfId="4" priority="10">
+    <cfRule type="expression" dxfId="1" priority="10">
       <formula>RIGHT($A9,5)="Total"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:K497">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>RIGHT($A15,5)="Total"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>